<commit_message>
c2 complete analysis for 3 questions commit
</commit_message>
<xml_diff>
--- a/results/Overall_score_analysis.xlsx
+++ b/results/Overall_score_analysis.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashvinn\Documents\GitHub\LLM_Interpretability_Research\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashvi\PycharmProjects\LLM_Interpretability_Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862D4C45-AF27-45A3-A434-EF8B2614A68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9BE966-7276-4881-903B-F40E857A8EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FE4610ED-2644-4B09-8F25-61DCA81DFAD7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
   <si>
     <t>ROUGE 1</t>
   </si>
@@ -226,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -284,6 +285,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -302,6 +304,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05E6529C-6372-131D-580A-D608EECB8A79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5124450" y="2844165"/>
+          <a:ext cx="5943600" cy="3566160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -350,7 +401,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -714,10 +765,442 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B1458-BA4B-4EAE-BCE9-A2C3FC37BD74}">
+  <dimension ref="A2:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="I2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0.59483278225686398</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.64655269326444698</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.50553126986247998</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E9" si="0">SUM(B4:D4)/3</f>
+        <v>0.5823055817945969</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.49316937027899199</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.47698746317606899</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.36475272781005202</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" ref="L4:L9" si="1">SUM(I4:K4)/3</f>
+        <v>0.44496985375503767</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.54188409095145496</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.57334421594170404</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.52062539037993405</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.54528456575769768</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.42775880358964002</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.412329251570974</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.400545281062894</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.41354444540783603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.60624233520883897</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.52304050584267003</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.53886560467152</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.55604948190767634</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.47743028387988401</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.35841287246797998</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.365873815127577</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40057232382514701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.49314375506108998</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.61496835266815697</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.58580376308082005</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5646386236033557</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.40643888290285701</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.43625146871410603</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.414710078328339</v>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.41913347664843403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.42342399871047198</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.50987605468068398</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.53264088454319802</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.48864697931145135</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.33864680802483799</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.341386222787537</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.37378752186971897</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.35127351756069797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.55091786261785403</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.59039433732525703</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.58511835040018301</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.57547685011443139</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.399703081000508</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.396547300699228</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.40898930253726201</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40174656141233261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.50920813121553699</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.261389725197615</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.31504409735246602</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:E11" si="2">SUM(B10:D10)/3</f>
+        <v>0.36188065125520597</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.41375574467480303</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.17964035837106099</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.22270358332376</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" ref="L10:L11" si="3">SUM(I10:K10)/3</f>
+        <v>0.27203322878987463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.50920813121553699</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.261389725197615</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.32918853922186198</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="2"/>
+        <v>0.36659546521167136</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.41375574467480303</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.17964035837106099</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.23607751536362601</v>
+      </c>
+      <c r="L11" s="8">
+        <f t="shared" si="3"/>
+        <v>0.27649120613649664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11" t="str">
+        <f>INDEX($A4:$A11, MATCH(MAX(B4:B11), B4:B11, 0))</f>
+        <v>v2-json</v>
+      </c>
+      <c r="C12" s="11" t="str">
+        <f t="shared" ref="C12:E12" si="4">INDEX($A4:$A11, MATCH(MAX(C4:C11), C4:C11, 0))</f>
+        <v>v0-unstruct</v>
+      </c>
+      <c r="D12" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>v2-html</v>
+      </c>
+      <c r="E12" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>v0-unstruct</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="11" t="str">
+        <f>INDEX($H4:$H11, MATCH(MAX(I4:I11), I4:I11, 0))</f>
+        <v>v0-unstruct</v>
+      </c>
+      <c r="J12" s="11" t="str">
+        <f t="shared" ref="J12:L12" si="5">INDEX($H4:$H11, MATCH(MAX(J4:J11), J4:J11, 0))</f>
+        <v>v0-unstruct</v>
+      </c>
+      <c r="K12" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>v2-html</v>
+      </c>
+      <c r="L12" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v>v0-unstruct</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="I2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:D11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:K11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA7B5C7-8A33-4FD1-986B-A27316631CA2}">
   <dimension ref="A2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -1073,7 +1556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525F6779-DD0B-49D7-B276-92B104E5F465}">
   <dimension ref="A2:L10"/>
   <sheetViews>
@@ -1417,7 +1900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA93D1B-782E-46E2-8D44-78C4206E258C}">
   <dimension ref="A2:L10"/>
   <sheetViews>
@@ -1769,7 +2252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3891B14-8636-44EC-9D3D-F5390233C3F1}">
   <dimension ref="A2:P12"/>
   <sheetViews>

</xml_diff>

<commit_message>
multiple question, and v2.1 commit
</commit_message>
<xml_diff>
--- a/results/Overall_score_analysis.xlsx
+++ b/results/Overall_score_analysis.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashvi\PycharmProjects\LLM_Interpretability_Research\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashvinn\Documents\GitHub\LLM_Interpretability_Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9BE966-7276-4881-903B-F40E857A8EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8BD27B-A26E-455D-A90A-6055161ABE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FE4610ED-2644-4B09-8F25-61DCA81DFAD7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="28">
   <si>
     <t>ROUGE 1</t>
   </si>
@@ -89,12 +91,48 @@
   <si>
     <t>biased docs working on  v2.1</t>
   </si>
+  <si>
+    <t>Clearly V2-toml and v2-custom3</t>
+  </si>
+  <si>
+    <t>is not good for large file</t>
+  </si>
+  <si>
+    <t>Q2 and Q3 docs is from a large file</t>
+  </si>
+  <si>
+    <t>v2.1-unstruct</t>
+  </si>
+  <si>
+    <t>v2.1-md</t>
+  </si>
+  <si>
+    <t>v2.1-toml</t>
+  </si>
+  <si>
+    <t>v2.1-json</t>
+  </si>
+  <si>
+    <t>v2.1-html</t>
+  </si>
+  <si>
+    <t>v2.1-custom1</t>
+  </si>
+  <si>
+    <t>v2.1-custom2</t>
+  </si>
+  <si>
+    <t>3 readings average</t>
+  </si>
+  <si>
+    <t>5 readings average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +194,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -227,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -279,13 +324,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,6 +350,103 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A097F33-309F-C05E-3FF4-EDF7D6CCE0FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="15065"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5495925" y="2571750"/>
+          <a:ext cx="6229350" cy="4400550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F62A7A-41A7-E9F9-FBA0-0F1F46A9F812}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5438774" y="2400299"/>
+          <a:ext cx="7477125" cy="4486275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -352,7 +495,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -401,7 +544,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -765,11 +908,819 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B1458-BA4B-4EAE-BCE9-A2C3FC37BD74}">
-  <dimension ref="A2:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC60521-07AC-4A58-A8B9-7F9C46143BF8}">
+  <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="I2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0.51418724135073102</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.65752632163805003</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.55939154720565198</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E9" si="0">SUM(B4:D4)/3</f>
+        <v>0.57703503673147771</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.40091393630130001</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.51272474295984105</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.40620984172796898</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" ref="L4:L9" si="1">SUM(I4:K4)/3</f>
+        <v>0.43994950699636998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.55198222628754201</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.60014959361070197</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.54181469908542201</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.56464883966122204</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.39034362504565001</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.46874817789145601</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.36825546704949302</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40911575666219968</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.36788831285463502</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.47544811103961698</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.48709566531558002</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.44347736306994401</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.30366929283857802</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.34937006414223498</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.30551202472927802</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.31951712723669701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.55506954624601601</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.58665307518651899</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.53484418308495696</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.55885560150583069</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.43330396859808601</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.46170557350449298</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.38452996480186002</v>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.42651316896814634</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.49393845375988199</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.61039622246798397</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.53539768188982395</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.54657745270589653</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.34208724030152599</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.42878683997834899</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.38893120410444798</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38660176146144098</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.59527838833603497</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.58861056357336194</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.56606340562149304</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.58331745251029665</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.43555739743058403</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.454614809398038</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.388651714988685</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.42627464060576897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.51839037596302595</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.61663256650652098</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.51998983545657895</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10" si="2">SUM(B10:D10)/3</f>
+        <v>0.55167092597537526</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.36481862147728</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.45340539500627303</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.345648093628183</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" ref="L10" si="3">SUM(I10:K10)/3</f>
+        <v>0.38795737003724534</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="11" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(B4:B10), B4:B10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="C11" s="11" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(C4:C10), C4:C10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+      <c r="D11" s="11" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(D4:D10), D4:D10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="E11" s="12" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(E4:E10), E4:E10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="11" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(I4:I10), I4:I10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="J11" s="11" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(J4:J10), J4:J10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+      <c r="K11" s="11" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(K4:K10), K4:K10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+      <c r="L11" s="19" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(L4:L10), L4:L10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="I2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:D10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:K10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E121A363-FC9D-421C-B4C0-C742E7C05D40}">
+  <dimension ref="A2:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="I2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0.52476084842883097</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.659995403586638</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.56065877676471898</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E9" si="0">SUM(B4:D4)/3</f>
+        <v>0.58180500959339598</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.41352638791785301</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.51394939636165105</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.40685355970444298</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" ref="L4:L9" si="1">SUM(I4:K4)/3</f>
+        <v>0.44477644799464899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.55089278223903404</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.59923595686182496</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.50660382284407002</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.55224418731497638</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.38647731514767802</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.46810744562600998</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.35373233839332102</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40277236638900304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.36602507637069298</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.47544811103961698</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.48371819016623901</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.44173045919218296</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.30318344456591101</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.34937006414223498</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.310327520531194</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.32096034307978</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.56169634202943897</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.588802498764184</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.54953289789552895</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.56667724622971727</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.43218772651798798</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.46125387313126698</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.42159584367664099</v>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.43834581444196535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.494464616121846</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.60926560640836103</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.580158865712192</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5612963627474663</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.3425136778142</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.42817672662989897</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.39993468716582897</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.39020836386997598</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.59527838833603497</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.59158993466698595</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.58074092535513899</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.58920308278605327</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.43555739743058403</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.46039219856219499</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.38528004809737798</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.42707654803005229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.51718654929439201</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.62033605154788096</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.52221834805516798</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10" si="2">SUM(B10:D10)/3</f>
+        <v>0.55324698296581365</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.36313417759496103</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.45433168219030501</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.34185549891256101</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" ref="L10" si="3">SUM(I10:K10)/3</f>
+        <v>0.3864404528992757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="11" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(B4:B10), B4:B10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="C11" s="11" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(C4:C10), C4:C10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+      <c r="D11" s="11" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(D4:D10), D4:D10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="E11" s="12" t="str">
+        <f>INDEX($A4:$A10, MATCH(MAX(E4:E10), E4:E10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="11" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(I4:I10), I4:I10, 0))</f>
+        <v>v2.1-custom1</v>
+      </c>
+      <c r="J11" s="11" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(J4:J10), J4:J10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+      <c r="K11" s="11" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(K4:K10), K4:K10, 0))</f>
+        <v>v2.1-json</v>
+      </c>
+      <c r="L11" s="19" t="str">
+        <f>INDEX($H4:$H10, MATCH(MAX(L4:L10), L4:L10, 0))</f>
+        <v>v2.1-unstruct</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="I2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:D10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:K10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B1458-BA4B-4EAE-BCE9-A2C3FC37BD74}">
+  <dimension ref="A2:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,16 +1735,16 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="I2" s="19" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1142,13 +2093,13 @@
         <f t="shared" si="5"/>
         <v>v2-html</v>
       </c>
-      <c r="L12" s="21" t="str">
+      <c r="L12" s="19" t="str">
         <f t="shared" si="5"/>
         <v>v0-unstruct</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="D15" s="20" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1160,6 +2111,21 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="20" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +2162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA7B5C7-8A33-4FD1-986B-A27316631CA2}">
   <dimension ref="A2:L15"/>
   <sheetViews>
@@ -1216,16 +2182,16 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="I2" s="19" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1556,7 +2522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525F6779-DD0B-49D7-B276-92B104E5F465}">
   <dimension ref="A2:L10"/>
   <sheetViews>
@@ -1576,16 +2542,16 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="I2" s="19" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1900,7 +2866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA93D1B-782E-46E2-8D44-78C4206E258C}">
   <dimension ref="A2:L10"/>
   <sheetViews>
@@ -1924,16 +2890,16 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="I2" s="19" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2252,7 +3218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3891B14-8636-44EC-9D3D-F5390233C3F1}">
   <dimension ref="A2:P12"/>
   <sheetViews>
@@ -2279,21 +3245,21 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>

</xml_diff>